<commit_message>
new docs, mri comparison script
</commit_message>
<xml_diff>
--- a/dpgmm_alpha15.4_bilateral_normals_conversions.xlsx
+++ b/dpgmm_alpha15.4_bilateral_normals_conversions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="51200" windowHeight="26740" tabRatio="500"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="51200" windowHeight="13360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="dpgmm_alpha15.4_bilateral_norma" sheetId="1" r:id="rId1"/>
@@ -525,13 +525,18 @@
   <dimension ref="A1:AQ15"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="X5" sqref="X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="23" max="23" width="15.7109375" customWidth="1"/>
+    <col min="24" max="24" width="22" customWidth="1"/>
+    <col min="25" max="25" width="18.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:43">
       <c r="A1" t="s">
@@ -2397,7 +2402,6 @@
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>